<commit_message>
1. Fix SimpleTest bugs; 2. Add hj71 problem; 3. Add longest palindromic substring problem;
</commit_message>
<xml_diff>
--- a/problems/longest-palindromic-substring/sol01.xlsx
+++ b/problems/longest-palindromic-substring/sol01.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\learning\leetcode\questions\longest-palindromic-substring\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\learning\leetcode\problems\longest-palindromic-substring\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9BE4F8D2-1005-439D-8687-EED17A775202}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FC0F919-C6DA-4094-8A8C-6ADA7D3A5377}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-5430" yWindow="-16590" windowWidth="24270" windowHeight="14940" xr2:uid="{1CFF41BE-A667-45E2-8A5A-7A9DD0B4AE4C}"/>
+    <workbookView xWindow="-4545" yWindow="-20040" windowWidth="24270" windowHeight="14940" xr2:uid="{1CFF41BE-A667-45E2-8A5A-7A9DD0B4AE4C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,19 +34,37 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="8">
   <si>
     <t>a</t>
   </si>
   <si>
     <t>b</t>
+  </si>
+  <si>
+    <t>input</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>j</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>f</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -61,8 +79,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -72,6 +96,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -88,15 +118,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -413,10 +449,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FCF8C51-1F88-4E65-89A8-F52714B8B7F5}">
-  <dimension ref="C3:I9"/>
+  <dimension ref="C3:J12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="C5" sqref="C5:J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -424,152 +460,228 @@
     <col min="1" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="E3" s="1">
-        <v>0</v>
-      </c>
-      <c r="F3" s="1">
-        <v>1</v>
-      </c>
-      <c r="G3" s="1">
+    <row r="3" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="1">
+      <c r="D3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="I3" s="1">
+      <c r="H3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="D5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="3">
+        <v>0</v>
+      </c>
+      <c r="F5" s="3">
+        <v>1</v>
+      </c>
+      <c r="G5" s="3">
+        <v>2</v>
+      </c>
+      <c r="H5" s="3">
+        <v>3</v>
+      </c>
+      <c r="I5" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="E4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C5" s="1">
-        <v>0</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E5" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="F5" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G5" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="H5" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="I5" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C6" s="1">
-        <v>1</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E6" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="F6" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="G6" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="H6" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="I6" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C7" s="1">
+      <c r="J5" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C7" s="3">
+        <v>0</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E7" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F7" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="G7" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="H7" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="I7" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J7" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C8" s="3">
+        <v>1</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E8" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="F8" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G8" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="H8" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I8" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J8" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C9" s="3">
         <v>2</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E7" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="F7" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="G7" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="H7" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="I7" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C8" s="1">
+      <c r="D9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="F9" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="G9" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H9" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I9" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="J9" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C10" s="3">
         <v>3</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E8" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="F8" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="G8" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="H8" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="I8" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C9" s="1">
+      <c r="D10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="F10" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="G10" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="H10" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="I10" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="J10" s="5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C11" s="3">
         <v>4</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E9" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="F9" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="G9" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="H9" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="I9" s="3" t="b">
+      <c r="D11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="F11" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="G11" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="H11" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="I11" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="J11" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C12" s="3">
+        <v>5</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="F12" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="G12" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="H12" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="I12" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J12" s="2" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>